<commit_message>
test-10 (negative vs positive)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-10.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-10.xlsx
@@ -153,6 +153,1014 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Positive flow</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'neg vs pos'!$O$4:$O$12</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>museums</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>parks</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>theatres</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>library</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cultureorg</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>musartschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'neg vs pos'!$Q$4:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.49660073586519959</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18580853340462811</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14071746644039071</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.332472789039854E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0640434127788856E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3842453401721149E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1910996975874061E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2833127489542253E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7897915119466892E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E746-4009-BEAA-8FC2C1AB7178}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Negative flow</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'neg vs pos'!$O$4:$O$12</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>museums</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>parks</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>theatres</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>library</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cultureorg</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>musartschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'neg vs pos'!$P$4:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.5196768833799518E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22460061112657481</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13437177712619999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3084750180750429E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0736916047546339E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9157363495510788E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4086790586132378E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8048554320054231E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43071646828343152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E746-4009-BEAA-8FC2C1AB7178}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="1619185935"/>
+        <c:axId val="1619191343"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1619185935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1619191343"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1619191343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1619185935"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,7 +1429,7 @@
   <dimension ref="C3:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J54"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,6 +1483,9 @@
       <c r="P4" s="3">
         <v>6.5196768833799518E-2</v>
       </c>
+      <c r="Q4" s="3">
+        <v>0.49660073586519959</v>
+      </c>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
@@ -489,13 +1500,20 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="3">
+        <v>77.338260453240693</v>
+      </c>
+      <c r="J5" s="3">
+        <v>172.95282178797291</v>
+      </c>
       <c r="O5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="P5" s="3">
         <v>0.22460061112657481</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.18580853340462811</v>
       </c>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
@@ -513,13 +1531,20 @@
         <f>H5+1</f>
         <v>2</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3">
+        <v>82.652965460637304</v>
+      </c>
+      <c r="J6" s="3">
+        <v>188.09633901320171</v>
+      </c>
       <c r="O6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="P6" s="3">
         <v>0.13437177712619999</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.14071746644039071</v>
       </c>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
@@ -537,14 +1562,21 @@
         <f t="shared" ref="H7:H54" si="1">H6+1</f>
         <v>3</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="3">
+        <v>83.46517638793955</v>
+      </c>
+      <c r="J7" s="3">
+        <v>186.84236732809219</v>
+      </c>
       <c r="O7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="P7" s="3">
         <v>1.3084750180750429E-2</v>
       </c>
+      <c r="Q7" s="3">
+        <v>2.332472789039854E-2</v>
+      </c>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -561,14 +1593,21 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="3">
+        <v>70.086108915840512</v>
+      </c>
+      <c r="J8" s="3">
+        <v>206.67166830006411</v>
+      </c>
       <c r="O8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="3">
         <v>1.0736916047546339E-2</v>
       </c>
+      <c r="Q8" s="3">
+        <v>7.0640434127788856E-3</v>
+      </c>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -585,14 +1624,21 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="3">
+        <v>76.58911673485899</v>
+      </c>
+      <c r="J9" s="3">
+        <v>179.29008847526441</v>
+      </c>
       <c r="O9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P9" s="3">
         <v>4.9157363495510788E-2</v>
       </c>
+      <c r="Q9" s="3">
+        <v>2.3842453401721149E-2</v>
+      </c>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -609,14 +1655,21 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="3">
+        <v>83.901045752951319</v>
+      </c>
+      <c r="J10" s="3">
+        <v>180.6447948135968</v>
+      </c>
       <c r="O10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="P10" s="3">
         <v>3.4086790586132378E-2</v>
       </c>
+      <c r="Q10" s="3">
+        <v>4.1910996975874061E-2</v>
+      </c>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -633,14 +1686,21 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="3">
+        <v>81.250049777021303</v>
+      </c>
+      <c r="J11" s="3">
+        <v>182.48737363165429</v>
+      </c>
       <c r="O11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P11" s="3">
         <v>3.8048554320054231E-2</v>
       </c>
+      <c r="Q11" s="3">
+        <v>4.2833127489542253E-2</v>
+      </c>
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -657,14 +1717,21 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3">
+        <v>81.219916692648709</v>
+      </c>
+      <c r="J12" s="3">
+        <v>193.60740165252221</v>
+      </c>
       <c r="O12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="P12" s="3">
         <v>0.43071646828343152</v>
       </c>
+      <c r="Q12" s="3">
+        <v>3.7897915119466892E-2</v>
+      </c>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -681,8 +1748,12 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="3">
+        <v>79.549545679272029</v>
+      </c>
+      <c r="J13" s="3">
+        <v>201.8719803518695</v>
+      </c>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
@@ -699,8 +1770,12 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="3">
+        <v>85.19736658507189</v>
+      </c>
+      <c r="J14" s="3">
+        <v>155.8397769599228</v>
+      </c>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -717,8 +1792,12 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="3">
+        <v>78.857523163240316</v>
+      </c>
+      <c r="J15" s="3">
+        <v>199.80224662490289</v>
+      </c>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
@@ -735,8 +1814,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3">
+        <v>83.703219726483823</v>
+      </c>
+      <c r="J16" s="3">
+        <v>188.72719016946661</v>
+      </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
@@ -753,8 +1836,12 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3">
+        <v>76.289450962470696</v>
+      </c>
+      <c r="J17" s="3">
+        <v>247.40968307888099</v>
+      </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -771,8 +1858,12 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="3">
+        <v>82.078374918760346</v>
+      </c>
+      <c r="J18" s="3">
+        <v>195.2632673882037</v>
+      </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
@@ -789,8 +1880,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="3">
+        <v>72.25000861706522</v>
+      </c>
+      <c r="J19" s="3">
+        <v>247.9136813117438</v>
+      </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
@@ -807,8 +1902,12 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="3">
+        <v>78.592697053565658</v>
+      </c>
+      <c r="J20" s="3">
+        <v>181.07134698377371</v>
+      </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -825,8 +1924,12 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="3">
+        <v>83.028428054309501</v>
+      </c>
+      <c r="J21" s="3">
+        <v>195.66269188342679</v>
+      </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
@@ -843,8 +1946,12 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3">
+        <v>82.065527299698388</v>
+      </c>
+      <c r="J22" s="3">
+        <v>159.10195317356249</v>
+      </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
@@ -861,8 +1968,12 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="3">
+        <v>78.861714605197605</v>
+      </c>
+      <c r="J23" s="3">
+        <v>198.00002810278639</v>
+      </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
@@ -879,8 +1990,12 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="3">
+        <v>81.378888050460631</v>
+      </c>
+      <c r="J24" s="3">
+        <v>145.72256528766479</v>
+      </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
@@ -897,8 +2012,12 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="I25" s="3">
+        <v>71.922875847106141</v>
+      </c>
+      <c r="J25" s="3">
+        <v>232.1153598857569</v>
+      </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -915,8 +2034,12 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="I26" s="3">
+        <v>79.647507322311867</v>
+      </c>
+      <c r="J26" s="3">
+        <v>188.14481151838569</v>
+      </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
@@ -933,8 +2056,12 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="3">
+        <v>81.056439813271226</v>
+      </c>
+      <c r="J27" s="3">
+        <v>147.54883325239581</v>
+      </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
@@ -951,8 +2078,12 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="3">
+        <v>67.521168866513591</v>
+      </c>
+      <c r="J28" s="3">
+        <v>223.03848075304319</v>
+      </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
@@ -969,8 +2100,12 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="3">
+        <v>76.74839422906274</v>
+      </c>
+      <c r="J29" s="3">
+        <v>167.9441748731287</v>
+      </c>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
@@ -987,8 +2122,12 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="3">
+        <v>73.832792004624267</v>
+      </c>
+      <c r="J30" s="3">
+        <v>227.77246329898989</v>
+      </c>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
@@ -1005,8 +2144,12 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="3">
+        <v>70.947340004464252</v>
+      </c>
+      <c r="J31" s="3">
+        <v>236.16953188515299</v>
+      </c>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
@@ -1023,8 +2166,12 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="I32" s="3">
+        <v>82.37997092234103</v>
+      </c>
+      <c r="J32" s="3">
+        <v>166.25405340026941</v>
+      </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
@@ -1041,8 +2188,12 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="3">
+        <v>85.166952852659932</v>
+      </c>
+      <c r="J33" s="3">
+        <v>167.4254692739745</v>
+      </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
@@ -1059,8 +2210,12 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="I34" s="3">
+        <v>73.736785609124865</v>
+      </c>
+      <c r="J34" s="3">
+        <v>218.5980863596846</v>
+      </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
@@ -1077,8 +2232,12 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="I35" s="3">
+        <v>79.141162044282382</v>
+      </c>
+      <c r="J35" s="3">
+        <v>194.28798754849001</v>
+      </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
@@ -1095,8 +2254,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="I36" s="3">
+        <v>82.217657876528961</v>
+      </c>
+      <c r="J36" s="3">
+        <v>152.7693071126404</v>
+      </c>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
@@ -1113,8 +2276,12 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="I37" s="3">
+        <v>77.113553517724128</v>
+      </c>
+      <c r="J37" s="3">
+        <v>203.55541182827699</v>
+      </c>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
@@ -1131,8 +2298,12 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="I38" s="3">
+        <v>79.245453535412011</v>
+      </c>
+      <c r="J38" s="3">
+        <v>184.27466008727069</v>
+      </c>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
@@ -1149,8 +2320,12 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="I39" s="3">
+        <v>77.30975862981191</v>
+      </c>
+      <c r="J39" s="3">
+        <v>174.33144138490181</v>
+      </c>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
@@ -1167,8 +2342,12 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="I40" s="3">
+        <v>70.258222049101008</v>
+      </c>
+      <c r="J40" s="3">
+        <v>241.04558892920349</v>
+      </c>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
@@ -1185,8 +2364,12 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="I41" s="3">
+        <v>80.176975990733283</v>
+      </c>
+      <c r="J41" s="3">
+        <v>153.50221182414629</v>
+      </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
@@ -1203,8 +2386,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
+      <c r="I42" s="3">
+        <v>74.854634821416369</v>
+      </c>
+      <c r="J42" s="3">
+        <v>235.76631902415841</v>
+      </c>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
@@ -1221,8 +2408,12 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+      <c r="I43" s="3">
+        <v>83.121132026160979</v>
+      </c>
+      <c r="J43" s="3">
+        <v>156.86798751903959</v>
+      </c>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
@@ -1239,8 +2430,12 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="I44" s="3">
+        <v>68.084805072899812</v>
+      </c>
+      <c r="J44" s="3">
+        <v>233.42378738121451</v>
+      </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
@@ -1257,8 +2452,12 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="I45" s="3">
+        <v>80.181727707391829</v>
+      </c>
+      <c r="J45" s="3">
+        <v>169.7965032082229</v>
+      </c>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
@@ -1275,8 +2474,12 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="I46" s="3">
+        <v>72.138414976893287</v>
+      </c>
+      <c r="J46" s="3">
+        <v>234.77878227810001</v>
+      </c>
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
@@ -1293,8 +2496,12 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="I47" s="3">
+        <v>78.422054884491743</v>
+      </c>
+      <c r="J47" s="3">
+        <v>186.75477426624309</v>
+      </c>
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
@@ -1311,8 +2518,12 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="I48" s="3">
+        <v>82.253603470540483</v>
+      </c>
+      <c r="J48" s="3">
+        <v>150.45274184731841</v>
+      </c>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
@@ -1329,8 +2540,12 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="I49" s="3">
+        <v>75.489364316385377</v>
+      </c>
+      <c r="J49" s="3">
+        <v>215.80604470876349</v>
+      </c>
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
@@ -1347,8 +2562,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
+      <c r="I50" s="3">
+        <v>85.599531555335545</v>
+      </c>
+      <c r="J50" s="3">
+        <v>164.64480031388359</v>
+      </c>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
@@ -1365,8 +2584,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+      <c r="I51" s="3">
+        <v>80.988698838854646</v>
+      </c>
+      <c r="J51" s="3">
+        <v>209.91224826986291</v>
+      </c>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
@@ -1383,8 +2606,12 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="I52" s="3">
+        <v>69.656291554763058</v>
+      </c>
+      <c r="J52" s="3">
+        <v>270.1018844208416</v>
+      </c>
     </row>
     <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
@@ -1401,8 +2628,12 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="I53" s="3">
+        <v>57.926353012140943</v>
+      </c>
+      <c r="J53" s="3">
+        <v>328.22779048343631</v>
+      </c>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
@@ -1419,8 +2650,12 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
+      <c r="I54" s="3">
+        <v>77.498727249748299</v>
+      </c>
+      <c r="J54" s="3">
+        <v>191.72570401011029</v>
+      </c>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
@@ -1437,13 +2672,13 @@
       <c r="H56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I56" s="3" t="e">
+      <c r="I56" s="3">
         <f>AVERAGE(I5:I54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J56" s="3" t="e">
+        <v>77.859874709856598</v>
+      </c>
+      <c r="J56" s="3">
         <f>AVERAGE(J5:J54)</f>
-        <v>#DIV/0!</v>
+        <v>196.68033014530948</v>
       </c>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.25">
@@ -1461,17 +2696,18 @@
       <c r="H57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="3" t="e">
+      <c r="I57" s="3">
         <f>_xlfn.STDEV.S(I5:I54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J57" s="3" t="e">
+        <v>5.5441744827448876</v>
+      </c>
+      <c r="J57" s="3">
         <f>_xlfn.STDEV.S(J5:J54)</f>
-        <v>#DIV/0!</v>
+        <v>35.715750895576541</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
positive flow (value driven)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-10.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-41-1 (positive flow).csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-41-1 (negative flow).csv)</t>
   </si>
 </sst>
 </file>
@@ -2721,13 +2724,15 @@
   <dimension ref="C3:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
     <col min="15" max="15" width="17.85546875" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" customWidth="1"/>
     <col min="17" max="17" width="13.7109375" customWidth="1"/>
@@ -2738,6 +2743,10 @@
         <v>18</v>
       </c>
       <c r="E3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1"/>
       <c r="O3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2756,96 +2765,186 @@
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="O4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="Q4" s="3">
+        <v>0.50818370109808642</v>
+      </c>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="3">
+        <v>111.1886580966647</v>
+      </c>
+      <c r="E5" s="3">
+        <v>268.10257471159412</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="O5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
+      <c r="Q5" s="3">
+        <v>0.11555709730215</v>
+      </c>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="3">
+        <v>100.99117335977699</v>
+      </c>
+      <c r="E6" s="3">
+        <v>303.02070298949093</v>
+      </c>
+      <c r="H6" s="2">
+        <f>H5+1</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="O6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+      <c r="Q6" s="3">
+        <v>0.19036362965674181</v>
+      </c>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3">
+        <v>108.40626016667871</v>
+      </c>
+      <c r="E7" s="3">
+        <v>281.52789721137452</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H54" si="1">H6+1</f>
+        <v>3</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="O7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
+      <c r="Q7" s="3">
+        <v>2.3630454130399159E-2</v>
+      </c>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3">
+        <v>111.0035159475302</v>
+      </c>
+      <c r="E8" s="3">
+        <v>282.65590098866647</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="O8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
+      <c r="Q8" s="3">
+        <v>6.8172152412313711E-2</v>
+      </c>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3">
+        <v>96.562943330575237</v>
+      </c>
+      <c r="E9" s="3">
+        <v>295.94806681374843</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
       <c r="O9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
+      <c r="Q9" s="3">
+        <v>5.4329727586011983E-2</v>
+      </c>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="3">
+        <v>100.0009339591232</v>
+      </c>
+      <c r="E10" s="3">
+        <v>329.0246097474797</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
       <c r="O10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="Q10" s="3">
+        <v>3.9763237814296977E-2</v>
+      </c>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3">
+        <v>105.3925044048778</v>
+      </c>
+      <c r="E11" s="3">
+        <v>302.04776601260693</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
@@ -2854,8 +2953,18 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="3">
+        <v>98.759612730051956</v>
+      </c>
+      <c r="E12" s="3">
+        <v>351.26896202463121</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
@@ -2864,360 +2973,802 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="3">
+        <v>107.2398732724089</v>
+      </c>
+      <c r="E13" s="3">
+        <v>298.20141019053642</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="3">
+        <v>104.29647019260619</v>
+      </c>
+      <c r="E14" s="3">
+        <v>320.25876922796618</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="3">
+        <v>109.4025134514736</v>
+      </c>
+      <c r="E15" s="3">
+        <v>285.10761703616248</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="3">
+        <v>105.703187280143</v>
+      </c>
+      <c r="E16" s="3">
+        <v>239.81572100969041</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="3">
+        <v>107.8717501202384</v>
+      </c>
+      <c r="E17" s="3">
+        <v>280.47865299487268</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="3">
+        <v>104.8422114182583</v>
+      </c>
+      <c r="E18" s="3">
+        <v>251.60192302941169</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="3">
+        <v>110.4056847502253</v>
+      </c>
+      <c r="E19" s="3">
+        <v>239.43213659460631</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="3">
+        <v>111.5020363101427</v>
+      </c>
+      <c r="E20" s="3">
+        <v>260.09208370969827</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="3">
+        <v>102.8923546528469</v>
+      </c>
+      <c r="E21" s="3">
+        <v>267.39962309387971</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="3">
+        <v>113.1808083028186</v>
+      </c>
+      <c r="E22" s="3">
+        <v>221.84037130399469</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="3">
+        <v>96.739023384561989</v>
+      </c>
+      <c r="E23" s="3">
+        <v>349.67685637034123</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="3">
+        <v>103.7866097705037</v>
+      </c>
+      <c r="E24" s="3">
+        <v>278.48645681927508</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="3">
+        <v>106.8190307088129</v>
+      </c>
+      <c r="E25" s="3">
+        <v>250.76721737567331</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="3">
+        <v>106.3460690421628</v>
+      </c>
+      <c r="E26" s="3">
+        <v>308.05668931641509</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="3">
+        <v>98.762797713182806</v>
+      </c>
+      <c r="E27" s="3">
+        <v>333.57149880470422</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="3">
+        <v>108.7893470642522</v>
+      </c>
+      <c r="E28" s="3">
+        <v>259.13094577386431</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="3">
+        <v>107.54328104511519</v>
+      </c>
+      <c r="E29" s="3">
+        <v>292.3653021551961</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="3">
+        <v>109.7295390622387</v>
+      </c>
+      <c r="E30" s="3">
+        <v>283.64753426651907</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="3">
+        <v>113.7437724186011</v>
+      </c>
+      <c r="E31" s="3">
+        <v>225.15151635668749</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="3">
+        <v>110.76586602591171</v>
+      </c>
+      <c r="E32" s="3">
+        <v>280.98294038683957</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="3">
+        <v>101.76153052429309</v>
+      </c>
+      <c r="E33" s="3">
+        <v>294.16151762995702</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="3">
+        <v>112.5750454432429</v>
+      </c>
+      <c r="E34" s="3">
+        <v>317.35819313122352</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="3">
+        <v>106.3330235664159</v>
+      </c>
+      <c r="E35" s="3">
+        <v>273.92426057117677</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="3">
+        <v>106.5141815052215</v>
+      </c>
+      <c r="E36" s="3">
+        <v>267.64904343363412</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="3">
+        <v>114.7238152929814</v>
+      </c>
+      <c r="E37" s="3">
+        <v>227.4860208215209</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="3">
+        <v>104.3182242288902</v>
+      </c>
+      <c r="E38" s="3">
+        <v>277.71552927655432</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="3">
+        <v>106.4565837114242</v>
+      </c>
+      <c r="E39" s="3">
+        <v>302.79092871477081</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="3">
+        <v>111.56766998934459</v>
+      </c>
+      <c r="E40" s="3">
+        <v>250.80979972610359</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="3">
+        <v>108.4022354564067</v>
+      </c>
+      <c r="E41" s="3">
+        <v>254.84968602169269</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="3">
+        <v>108.5060566120588</v>
+      </c>
+      <c r="E42" s="3">
+        <v>328.56463600386701</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="3">
+        <v>102.91162961117639</v>
+      </c>
+      <c r="E43" s="3">
+        <v>289.8196377990696</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="3">
+        <v>99.291107956038331</v>
+      </c>
+      <c r="E44" s="3">
+        <v>330.28396437490852</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="3">
+        <v>103.4622585109128</v>
+      </c>
+      <c r="E45" s="3">
+        <v>279.21252099251672</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="3">
+        <v>103.06473362566889</v>
+      </c>
+      <c r="E46" s="3">
+        <v>277.95901250858259</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="3">
+        <v>113.4511271620887</v>
+      </c>
+      <c r="E47" s="3">
+        <v>265.26836646672638</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="3">
+        <v>107.9528562445641</v>
+      </c>
+      <c r="E48" s="3">
+        <v>258.0884023290123</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="3">
+        <v>102.0278646274611</v>
+      </c>
+      <c r="E49" s="3">
+        <v>286.57594568030169</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="3">
+        <v>103.0870890389493</v>
+      </c>
+      <c r="E50" s="3">
+        <v>321.31910068929471</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="3">
+        <v>104.6742553534328</v>
+      </c>
+      <c r="E51" s="3">
+        <v>289.15684188838179</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="3">
+        <v>110.9251952543981</v>
+      </c>
+      <c r="E52" s="3">
+        <v>266.42022705352178</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="3">
+        <v>101.7129349045741</v>
+      </c>
+      <c r="E53" s="3">
+        <v>335.83373690511883</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="3">
+        <v>105.4802777347512</v>
+      </c>
+      <c r="E54" s="3">
+        <v>307.04783719704812</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="3" t="e">
+      <c r="D56" s="3">
         <f>AVERAGE(D5:D54)</f>
+        <v>106.23735048672161</v>
+      </c>
+      <c r="E56" s="3">
+        <f>AVERAGE(E5:E54)</f>
+        <v>284.83913911061819</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I56" s="3" t="e">
+        <f>AVERAGE(I5:I54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E56" s="3" t="e">
-        <f>AVERAGE(E5:E54)</f>
+      <c r="J56" s="3" t="e">
+        <f>AVERAGE(J5:J54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="3" t="e">
+      <c r="D57" s="3">
         <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>4.566783770153914</v>
+      </c>
+      <c r="E57" s="3">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>31.558725628405536</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I57" s="3" t="e">
+        <f>_xlfn.STDEV.S(I5:I54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E57" s="3" t="e">
-        <f>_xlfn.STDEV.S(E5:E54)</f>
+      <c r="J57" s="3" t="e">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>